<commit_message>
Created cleaned table Voter. All tables saved in .xlsx file.
</commit_message>
<xml_diff>
--- a/data/au_marriage_cleaned.xlsx
+++ b/data/au_marriage_cleaned.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Division" sheetId="1" r:id="rId1"/>
     <sheet name="Voting Results" sheetId="2" r:id="rId2"/>
+    <sheet name="Voter" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="171">
   <si>
     <t>division</t>
   </si>
@@ -510,6 +511,24 @@
   </si>
   <si>
     <t>total_count</t>
+  </si>
+  <si>
+    <t>resp_clear_count</t>
+  </si>
+  <si>
+    <t>resp_clear_percent</t>
+  </si>
+  <si>
+    <t>resp_not_clear_count</t>
+  </si>
+  <si>
+    <t>resp_not_clear_percent</t>
+  </si>
+  <si>
+    <t>non_resp_count</t>
+  </si>
+  <si>
+    <t>non_resp_percent</t>
   </si>
 </sst>
 </file>
@@ -5117,4 +5136,3943 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H151"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>84079</v>
+      </c>
+      <c r="C2">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="D2">
+        <v>247</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>20928</v>
+      </c>
+      <c r="G2">
+        <v>19.9</v>
+      </c>
+      <c r="H2">
+        <v>105254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>85137</v>
+      </c>
+      <c r="C3">
+        <v>77.8</v>
+      </c>
+      <c r="D3">
+        <v>226</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <v>24008</v>
+      </c>
+      <c r="G3">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>109371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>86158</v>
+      </c>
+      <c r="C4">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>244</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <v>19973</v>
+      </c>
+      <c r="G4">
+        <v>18.8</v>
+      </c>
+      <c r="H4">
+        <v>106375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>88840</v>
+      </c>
+      <c r="C5">
+        <v>84.5</v>
+      </c>
+      <c r="D5">
+        <v>212</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>16038</v>
+      </c>
+      <c r="G5">
+        <v>15.3</v>
+      </c>
+      <c r="H5">
+        <v>105090</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>78332</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>220</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>25883</v>
+      </c>
+      <c r="G6">
+        <v>24.8</v>
+      </c>
+      <c r="H6">
+        <v>104435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>88608</v>
+      </c>
+      <c r="C7">
+        <v>83.5</v>
+      </c>
+      <c r="D7">
+        <v>202</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <v>17261</v>
+      </c>
+      <c r="G7">
+        <v>16.3</v>
+      </c>
+      <c r="H7">
+        <v>106071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>89870</v>
+      </c>
+      <c r="C8">
+        <v>77.8</v>
+      </c>
+      <c r="D8">
+        <v>285</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>25342</v>
+      </c>
+      <c r="G8">
+        <v>21.9</v>
+      </c>
+      <c r="H8">
+        <v>115497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>79573</v>
+      </c>
+      <c r="C9">
+        <v>73.7</v>
+      </c>
+      <c r="D9">
+        <v>263</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>28180</v>
+      </c>
+      <c r="G9">
+        <v>26.1</v>
+      </c>
+      <c r="H9">
+        <v>108016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>86309</v>
+      </c>
+      <c r="C10">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <v>229</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>18713</v>
+      </c>
+      <c r="G10">
+        <v>17.8</v>
+      </c>
+      <c r="H10">
+        <v>105251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>95810</v>
+      </c>
+      <c r="C11">
+        <v>79</v>
+      </c>
+      <c r="D11">
+        <v>315</v>
+      </c>
+      <c r="E11">
+        <v>0.3</v>
+      </c>
+      <c r="F11">
+        <v>25197</v>
+      </c>
+      <c r="G11">
+        <v>20.8</v>
+      </c>
+      <c r="H11">
+        <v>121322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>92746</v>
+      </c>
+      <c r="C12">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="D12">
+        <v>268</v>
+      </c>
+      <c r="E12">
+        <v>0.2</v>
+      </c>
+      <c r="F12">
+        <v>20607</v>
+      </c>
+      <c r="G12">
+        <v>18.1</v>
+      </c>
+      <c r="H12">
+        <v>113621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>90462</v>
+      </c>
+      <c r="C13">
+        <v>78.7</v>
+      </c>
+      <c r="D13">
+        <v>255</v>
+      </c>
+      <c r="E13">
+        <v>0.2</v>
+      </c>
+      <c r="F13">
+        <v>24275</v>
+      </c>
+      <c r="G13">
+        <v>21.1</v>
+      </c>
+      <c r="H13">
+        <v>114992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>88149</v>
+      </c>
+      <c r="C14">
+        <v>79.7</v>
+      </c>
+      <c r="D14">
+        <v>249</v>
+      </c>
+      <c r="E14">
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>22139</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>110537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>87729</v>
+      </c>
+      <c r="C15">
+        <v>77.2</v>
+      </c>
+      <c r="D15">
+        <v>277</v>
+      </c>
+      <c r="E15">
+        <v>0.2</v>
+      </c>
+      <c r="F15">
+        <v>25669</v>
+      </c>
+      <c r="G15">
+        <v>22.6</v>
+      </c>
+      <c r="H15">
+        <v>113675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>76629</v>
+      </c>
+      <c r="C16">
+        <v>72.2</v>
+      </c>
+      <c r="D16">
+        <v>228</v>
+      </c>
+      <c r="E16">
+        <v>0.2</v>
+      </c>
+      <c r="F16">
+        <v>29251</v>
+      </c>
+      <c r="G16">
+        <v>27.6</v>
+      </c>
+      <c r="H16">
+        <v>106108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>95708</v>
+      </c>
+      <c r="C17">
+        <v>80.3</v>
+      </c>
+      <c r="D17">
+        <v>303</v>
+      </c>
+      <c r="E17">
+        <v>0.3</v>
+      </c>
+      <c r="F17">
+        <v>23109</v>
+      </c>
+      <c r="G17">
+        <v>19.4</v>
+      </c>
+      <c r="H17">
+        <v>119120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>91637</v>
+      </c>
+      <c r="C18">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>136</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+      <c r="F18">
+        <v>16074</v>
+      </c>
+      <c r="G18">
+        <v>14.9</v>
+      </c>
+      <c r="H18">
+        <v>107847</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>81996</v>
+      </c>
+      <c r="C19">
+        <v>76.3</v>
+      </c>
+      <c r="D19">
+        <v>217</v>
+      </c>
+      <c r="E19">
+        <v>0.2</v>
+      </c>
+      <c r="F19">
+        <v>25253</v>
+      </c>
+      <c r="G19">
+        <v>23.5</v>
+      </c>
+      <c r="H19">
+        <v>107466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>87895</v>
+      </c>
+      <c r="C20">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="D20">
+        <v>185</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>17038</v>
+      </c>
+      <c r="G20">
+        <v>16.2</v>
+      </c>
+      <c r="H20">
+        <v>105118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>87555</v>
+      </c>
+      <c r="C21">
+        <v>78.7</v>
+      </c>
+      <c r="D21">
+        <v>213</v>
+      </c>
+      <c r="E21">
+        <v>0.2</v>
+      </c>
+      <c r="F21">
+        <v>23457</v>
+      </c>
+      <c r="G21">
+        <v>21.1</v>
+      </c>
+      <c r="H21">
+        <v>111225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>91860</v>
+      </c>
+      <c r="C22">
+        <v>78.3</v>
+      </c>
+      <c r="D22">
+        <v>251</v>
+      </c>
+      <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>25253</v>
+      </c>
+      <c r="G22">
+        <v>21.5</v>
+      </c>
+      <c r="H22">
+        <v>117364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>87807</v>
+      </c>
+      <c r="C23">
+        <v>79.5</v>
+      </c>
+      <c r="D23">
+        <v>225</v>
+      </c>
+      <c r="E23">
+        <v>0.2</v>
+      </c>
+      <c r="F23">
+        <v>22399</v>
+      </c>
+      <c r="G23">
+        <v>20.3</v>
+      </c>
+      <c r="H23">
+        <v>110431</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>87366</v>
+      </c>
+      <c r="C24">
+        <v>76.3</v>
+      </c>
+      <c r="D24">
+        <v>234</v>
+      </c>
+      <c r="E24">
+        <v>0.2</v>
+      </c>
+      <c r="F24">
+        <v>26955</v>
+      </c>
+      <c r="G24">
+        <v>23.5</v>
+      </c>
+      <c r="H24">
+        <v>114555</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>92955</v>
+      </c>
+      <c r="C25">
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <v>316</v>
+      </c>
+      <c r="E25">
+        <v>0.3</v>
+      </c>
+      <c r="F25">
+        <v>21426</v>
+      </c>
+      <c r="G25">
+        <v>18.7</v>
+      </c>
+      <c r="H25">
+        <v>114697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>83230</v>
+      </c>
+      <c r="C26">
+        <v>75.2</v>
+      </c>
+      <c r="D26">
+        <v>228</v>
+      </c>
+      <c r="E26">
+        <v>0.2</v>
+      </c>
+      <c r="F26">
+        <v>27271</v>
+      </c>
+      <c r="G26">
+        <v>24.6</v>
+      </c>
+      <c r="H26">
+        <v>110729</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>91680</v>
+      </c>
+      <c r="C27">
+        <v>83.8</v>
+      </c>
+      <c r="D27">
+        <v>208</v>
+      </c>
+      <c r="E27">
+        <v>0.2</v>
+      </c>
+      <c r="F27">
+        <v>17500</v>
+      </c>
+      <c r="G27">
+        <v>16</v>
+      </c>
+      <c r="H27">
+        <v>109388</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>87958</v>
+      </c>
+      <c r="C28">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="D28">
+        <v>235</v>
+      </c>
+      <c r="E28">
+        <v>0.2</v>
+      </c>
+      <c r="F28">
+        <v>18490</v>
+      </c>
+      <c r="G28">
+        <v>17.3</v>
+      </c>
+      <c r="H28">
+        <v>106683</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>83113</v>
+      </c>
+      <c r="C29">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="D29">
+        <v>242</v>
+      </c>
+      <c r="E29">
+        <v>0.2</v>
+      </c>
+      <c r="F29">
+        <v>23721</v>
+      </c>
+      <c r="G29">
+        <v>22.2</v>
+      </c>
+      <c r="H29">
+        <v>107076</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>85764</v>
+      </c>
+      <c r="C30">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="D30">
+        <v>176</v>
+      </c>
+      <c r="E30">
+        <v>0.2</v>
+      </c>
+      <c r="F30">
+        <v>19436</v>
+      </c>
+      <c r="G30">
+        <v>18.4</v>
+      </c>
+      <c r="H30">
+        <v>105376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>95157</v>
+      </c>
+      <c r="C31">
+        <v>82.5</v>
+      </c>
+      <c r="D31">
+        <v>232</v>
+      </c>
+      <c r="E31">
+        <v>0.2</v>
+      </c>
+      <c r="F31">
+        <v>19970</v>
+      </c>
+      <c r="G31">
+        <v>17.3</v>
+      </c>
+      <c r="H31">
+        <v>115359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>84932</v>
+      </c>
+      <c r="C32">
+        <v>76.7</v>
+      </c>
+      <c r="D32">
+        <v>256</v>
+      </c>
+      <c r="E32">
+        <v>0.2</v>
+      </c>
+      <c r="F32">
+        <v>25581</v>
+      </c>
+      <c r="G32">
+        <v>23.1</v>
+      </c>
+      <c r="H32">
+        <v>110769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>90286</v>
+      </c>
+      <c r="C33">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="D33">
+        <v>193</v>
+      </c>
+      <c r="E33">
+        <v>0.2</v>
+      </c>
+      <c r="F33">
+        <v>17538</v>
+      </c>
+      <c r="G33">
+        <v>16.2</v>
+      </c>
+      <c r="H33">
+        <v>108017</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>93670</v>
+      </c>
+      <c r="C34">
+        <v>78.3</v>
+      </c>
+      <c r="D34">
+        <v>291</v>
+      </c>
+      <c r="E34">
+        <v>0.2</v>
+      </c>
+      <c r="F34">
+        <v>25645</v>
+      </c>
+      <c r="G34">
+        <v>21.4</v>
+      </c>
+      <c r="H34">
+        <v>119606</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>78516</v>
+      </c>
+      <c r="C35">
+        <v>72.3</v>
+      </c>
+      <c r="D35">
+        <v>241</v>
+      </c>
+      <c r="E35">
+        <v>0.2</v>
+      </c>
+      <c r="F35">
+        <v>29777</v>
+      </c>
+      <c r="G35">
+        <v>27.4</v>
+      </c>
+      <c r="H35">
+        <v>108534</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>76337</v>
+      </c>
+      <c r="C36">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="D36">
+        <v>197</v>
+      </c>
+      <c r="E36">
+        <v>0.2</v>
+      </c>
+      <c r="F36">
+        <v>25757</v>
+      </c>
+      <c r="G36">
+        <v>25.2</v>
+      </c>
+      <c r="H36">
+        <v>102291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>92974</v>
+      </c>
+      <c r="C37">
+        <v>79.09999999999999</v>
+      </c>
+      <c r="D37">
+        <v>279</v>
+      </c>
+      <c r="E37">
+        <v>0.2</v>
+      </c>
+      <c r="F37">
+        <v>24264</v>
+      </c>
+      <c r="G37">
+        <v>20.6</v>
+      </c>
+      <c r="H37">
+        <v>117517</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>82628</v>
+      </c>
+      <c r="C38">
+        <v>77.5</v>
+      </c>
+      <c r="D38">
+        <v>203</v>
+      </c>
+      <c r="E38">
+        <v>0.2</v>
+      </c>
+      <c r="F38">
+        <v>23786</v>
+      </c>
+      <c r="G38">
+        <v>22.3</v>
+      </c>
+      <c r="H38">
+        <v>106617</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>92216</v>
+      </c>
+      <c r="C39">
+        <v>80</v>
+      </c>
+      <c r="D39">
+        <v>274</v>
+      </c>
+      <c r="E39">
+        <v>0.2</v>
+      </c>
+      <c r="F39">
+        <v>22719</v>
+      </c>
+      <c r="G39">
+        <v>19.7</v>
+      </c>
+      <c r="H39">
+        <v>115209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>86641</v>
+      </c>
+      <c r="C40">
+        <v>77</v>
+      </c>
+      <c r="D40">
+        <v>265</v>
+      </c>
+      <c r="E40">
+        <v>0.2</v>
+      </c>
+      <c r="F40">
+        <v>25632</v>
+      </c>
+      <c r="G40">
+        <v>22.8</v>
+      </c>
+      <c r="H40">
+        <v>112538</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>89303</v>
+      </c>
+      <c r="C41">
+        <v>81.2</v>
+      </c>
+      <c r="D41">
+        <v>231</v>
+      </c>
+      <c r="E41">
+        <v>0.2</v>
+      </c>
+      <c r="F41">
+        <v>20431</v>
+      </c>
+      <c r="G41">
+        <v>18.6</v>
+      </c>
+      <c r="H41">
+        <v>109965</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>92291</v>
+      </c>
+      <c r="C42">
+        <v>82.2</v>
+      </c>
+      <c r="D42">
+        <v>255</v>
+      </c>
+      <c r="E42">
+        <v>0.2</v>
+      </c>
+      <c r="F42">
+        <v>19675</v>
+      </c>
+      <c r="G42">
+        <v>17.5</v>
+      </c>
+      <c r="H42">
+        <v>112221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>91004</v>
+      </c>
+      <c r="C43">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="D43">
+        <v>146</v>
+      </c>
+      <c r="E43">
+        <v>0.1</v>
+      </c>
+      <c r="F43">
+        <v>22093</v>
+      </c>
+      <c r="G43">
+        <v>19.5</v>
+      </c>
+      <c r="H43">
+        <v>113243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
+        <v>86659</v>
+      </c>
+      <c r="C44">
+        <v>83.8</v>
+      </c>
+      <c r="D44">
+        <v>172</v>
+      </c>
+      <c r="E44">
+        <v>0.2</v>
+      </c>
+      <c r="F44">
+        <v>16630</v>
+      </c>
+      <c r="G44">
+        <v>16.1</v>
+      </c>
+      <c r="H44">
+        <v>103461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>82075</v>
+      </c>
+      <c r="C45">
+        <v>76.8</v>
+      </c>
+      <c r="D45">
+        <v>205</v>
+      </c>
+      <c r="E45">
+        <v>0.2</v>
+      </c>
+      <c r="F45">
+        <v>24634</v>
+      </c>
+      <c r="G45">
+        <v>23</v>
+      </c>
+      <c r="H45">
+        <v>106914</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46">
+        <v>85689</v>
+      </c>
+      <c r="C46">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="D46">
+        <v>162</v>
+      </c>
+      <c r="E46">
+        <v>0.2</v>
+      </c>
+      <c r="F46">
+        <v>18121</v>
+      </c>
+      <c r="G46">
+        <v>17.4</v>
+      </c>
+      <c r="H46">
+        <v>103972</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <v>83426</v>
+      </c>
+      <c r="C47">
+        <v>73.8</v>
+      </c>
+      <c r="D47">
+        <v>269</v>
+      </c>
+      <c r="E47">
+        <v>0.2</v>
+      </c>
+      <c r="F47">
+        <v>29282</v>
+      </c>
+      <c r="G47">
+        <v>25.9</v>
+      </c>
+      <c r="H47">
+        <v>112977</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>92441</v>
+      </c>
+      <c r="C48">
+        <v>79.8</v>
+      </c>
+      <c r="D48">
+        <v>276</v>
+      </c>
+      <c r="E48">
+        <v>0.2</v>
+      </c>
+      <c r="F48">
+        <v>23064</v>
+      </c>
+      <c r="G48">
+        <v>19.9</v>
+      </c>
+      <c r="H48">
+        <v>115781</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49">
+        <v>78185</v>
+      </c>
+      <c r="C49">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="D49">
+        <v>234</v>
+      </c>
+      <c r="E49">
+        <v>0.2</v>
+      </c>
+      <c r="F49">
+        <v>17664</v>
+      </c>
+      <c r="G49">
+        <v>18.4</v>
+      </c>
+      <c r="H49">
+        <v>96083</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50">
+        <v>93018</v>
+      </c>
+      <c r="C50">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="D50">
+        <v>333</v>
+      </c>
+      <c r="E50">
+        <v>0.3</v>
+      </c>
+      <c r="F50">
+        <v>20923</v>
+      </c>
+      <c r="G50">
+        <v>18.3</v>
+      </c>
+      <c r="H50">
+        <v>114274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51">
+        <v>93289</v>
+      </c>
+      <c r="C51">
+        <v>83.7</v>
+      </c>
+      <c r="D51">
+        <v>287</v>
+      </c>
+      <c r="E51">
+        <v>0.3</v>
+      </c>
+      <c r="F51">
+        <v>17901</v>
+      </c>
+      <c r="G51">
+        <v>16.1</v>
+      </c>
+      <c r="H51">
+        <v>111477</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>92264</v>
+      </c>
+      <c r="C52">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="D52">
+        <v>333</v>
+      </c>
+      <c r="E52">
+        <v>0.3</v>
+      </c>
+      <c r="F52">
+        <v>19360</v>
+      </c>
+      <c r="G52">
+        <v>17.3</v>
+      </c>
+      <c r="H52">
+        <v>111957</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>73847</v>
+      </c>
+      <c r="C53">
+        <v>77.40000000000001</v>
+      </c>
+      <c r="D53">
+        <v>257</v>
+      </c>
+      <c r="E53">
+        <v>0.3</v>
+      </c>
+      <c r="F53">
+        <v>21261</v>
+      </c>
+      <c r="G53">
+        <v>22.3</v>
+      </c>
+      <c r="H53">
+        <v>95365</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54">
+        <v>87662</v>
+      </c>
+      <c r="C54">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="D54">
+        <v>331</v>
+      </c>
+      <c r="E54">
+        <v>0.3</v>
+      </c>
+      <c r="F54">
+        <v>23588</v>
+      </c>
+      <c r="G54">
+        <v>21.1</v>
+      </c>
+      <c r="H54">
+        <v>111581</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55">
+        <v>88103</v>
+      </c>
+      <c r="C55">
+        <v>83.7</v>
+      </c>
+      <c r="D55">
+        <v>316</v>
+      </c>
+      <c r="E55">
+        <v>0.3</v>
+      </c>
+      <c r="F55">
+        <v>16807</v>
+      </c>
+      <c r="G55">
+        <v>16</v>
+      </c>
+      <c r="H55">
+        <v>105226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56">
+        <v>80292</v>
+      </c>
+      <c r="C56">
+        <v>82.09999999999999</v>
+      </c>
+      <c r="D56">
+        <v>271</v>
+      </c>
+      <c r="E56">
+        <v>0.3</v>
+      </c>
+      <c r="F56">
+        <v>17188</v>
+      </c>
+      <c r="G56">
+        <v>17.6</v>
+      </c>
+      <c r="H56">
+        <v>97751</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <v>97431</v>
+      </c>
+      <c r="C57">
+        <v>84.8</v>
+      </c>
+      <c r="D57">
+        <v>326</v>
+      </c>
+      <c r="E57">
+        <v>0.3</v>
+      </c>
+      <c r="F57">
+        <v>17123</v>
+      </c>
+      <c r="G57">
+        <v>14.9</v>
+      </c>
+      <c r="H57">
+        <v>114880</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58">
+        <v>92523</v>
+      </c>
+      <c r="C58">
+        <v>83.3</v>
+      </c>
+      <c r="D58">
+        <v>359</v>
+      </c>
+      <c r="E58">
+        <v>0.3</v>
+      </c>
+      <c r="F58">
+        <v>18255</v>
+      </c>
+      <c r="G58">
+        <v>16.4</v>
+      </c>
+      <c r="H58">
+        <v>111137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59">
+        <v>84437</v>
+      </c>
+      <c r="C59">
+        <v>84.40000000000001</v>
+      </c>
+      <c r="D59">
+        <v>276</v>
+      </c>
+      <c r="E59">
+        <v>0.3</v>
+      </c>
+      <c r="F59">
+        <v>15389</v>
+      </c>
+      <c r="G59">
+        <v>15.4</v>
+      </c>
+      <c r="H59">
+        <v>100102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60">
+        <v>87311</v>
+      </c>
+      <c r="C60">
+        <v>81.7</v>
+      </c>
+      <c r="D60">
+        <v>285</v>
+      </c>
+      <c r="E60">
+        <v>0.3</v>
+      </c>
+      <c r="F60">
+        <v>19322</v>
+      </c>
+      <c r="G60">
+        <v>18.1</v>
+      </c>
+      <c r="H60">
+        <v>106918</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61">
+        <v>97566</v>
+      </c>
+      <c r="C61">
+        <v>81.8</v>
+      </c>
+      <c r="D61">
+        <v>336</v>
+      </c>
+      <c r="E61">
+        <v>0.3</v>
+      </c>
+      <c r="F61">
+        <v>21407</v>
+      </c>
+      <c r="G61">
+        <v>17.9</v>
+      </c>
+      <c r="H61">
+        <v>119309</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>91110</v>
+      </c>
+      <c r="C62">
+        <v>82</v>
+      </c>
+      <c r="D62">
+        <v>278</v>
+      </c>
+      <c r="E62">
+        <v>0.3</v>
+      </c>
+      <c r="F62">
+        <v>19771</v>
+      </c>
+      <c r="G62">
+        <v>17.8</v>
+      </c>
+      <c r="H62">
+        <v>111159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63">
+        <v>85106</v>
+      </c>
+      <c r="C63">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="D63">
+        <v>338</v>
+      </c>
+      <c r="E63">
+        <v>0.3</v>
+      </c>
+      <c r="F63">
+        <v>20370</v>
+      </c>
+      <c r="G63">
+        <v>19.3</v>
+      </c>
+      <c r="H63">
+        <v>105814</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>91389</v>
+      </c>
+      <c r="C64">
+        <v>85.8</v>
+      </c>
+      <c r="D64">
+        <v>238</v>
+      </c>
+      <c r="E64">
+        <v>0.2</v>
+      </c>
+      <c r="F64">
+        <v>14857</v>
+      </c>
+      <c r="G64">
+        <v>14</v>
+      </c>
+      <c r="H64">
+        <v>106484</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65">
+        <v>93421</v>
+      </c>
+      <c r="C65">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="D65">
+        <v>347</v>
+      </c>
+      <c r="E65">
+        <v>0.3</v>
+      </c>
+      <c r="F65">
+        <v>27479</v>
+      </c>
+      <c r="G65">
+        <v>22.7</v>
+      </c>
+      <c r="H65">
+        <v>121247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66">
+        <v>89434</v>
+      </c>
+      <c r="C66">
+        <v>84.2</v>
+      </c>
+      <c r="D66">
+        <v>180</v>
+      </c>
+      <c r="E66">
+        <v>0.2</v>
+      </c>
+      <c r="F66">
+        <v>16615</v>
+      </c>
+      <c r="G66">
+        <v>15.6</v>
+      </c>
+      <c r="H66">
+        <v>106229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67">
+        <v>93022</v>
+      </c>
+      <c r="C67">
+        <v>76.5</v>
+      </c>
+      <c r="D67">
+        <v>289</v>
+      </c>
+      <c r="E67">
+        <v>0.2</v>
+      </c>
+      <c r="F67">
+        <v>28260</v>
+      </c>
+      <c r="G67">
+        <v>23.2</v>
+      </c>
+      <c r="H67">
+        <v>121571</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68">
+        <v>80510</v>
+      </c>
+      <c r="C68">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="D68">
+        <v>303</v>
+      </c>
+      <c r="E68">
+        <v>0.3</v>
+      </c>
+      <c r="F68">
+        <v>19732</v>
+      </c>
+      <c r="G68">
+        <v>19.6</v>
+      </c>
+      <c r="H68">
+        <v>100545</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69">
+        <v>86488</v>
+      </c>
+      <c r="C69">
+        <v>81.8</v>
+      </c>
+      <c r="D69">
+        <v>324</v>
+      </c>
+      <c r="E69">
+        <v>0.3</v>
+      </c>
+      <c r="F69">
+        <v>18934</v>
+      </c>
+      <c r="G69">
+        <v>17.9</v>
+      </c>
+      <c r="H69">
+        <v>105746</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70">
+        <v>86708</v>
+      </c>
+      <c r="C70">
+        <v>80.5</v>
+      </c>
+      <c r="D70">
+        <v>275</v>
+      </c>
+      <c r="E70">
+        <v>0.3</v>
+      </c>
+      <c r="F70">
+        <v>20692</v>
+      </c>
+      <c r="G70">
+        <v>19.2</v>
+      </c>
+      <c r="H70">
+        <v>107675</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71">
+        <v>88551</v>
+      </c>
+      <c r="C71">
+        <v>85</v>
+      </c>
+      <c r="D71">
+        <v>255</v>
+      </c>
+      <c r="E71">
+        <v>0.2</v>
+      </c>
+      <c r="F71">
+        <v>15363</v>
+      </c>
+      <c r="G71">
+        <v>14.7</v>
+      </c>
+      <c r="H71">
+        <v>104169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72">
+        <v>86321</v>
+      </c>
+      <c r="C72">
+        <v>85.7</v>
+      </c>
+      <c r="D72">
+        <v>231</v>
+      </c>
+      <c r="E72">
+        <v>0.2</v>
+      </c>
+      <c r="F72">
+        <v>14147</v>
+      </c>
+      <c r="G72">
+        <v>14</v>
+      </c>
+      <c r="H72">
+        <v>100699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73">
+        <v>100491</v>
+      </c>
+      <c r="C73">
+        <v>76.7</v>
+      </c>
+      <c r="D73">
+        <v>345</v>
+      </c>
+      <c r="E73">
+        <v>0.3</v>
+      </c>
+      <c r="F73">
+        <v>30127</v>
+      </c>
+      <c r="G73">
+        <v>23</v>
+      </c>
+      <c r="H73">
+        <v>130963</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74">
+        <v>91633</v>
+      </c>
+      <c r="C74">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="D74">
+        <v>268</v>
+      </c>
+      <c r="E74">
+        <v>0.2</v>
+      </c>
+      <c r="F74">
+        <v>19002</v>
+      </c>
+      <c r="G74">
+        <v>17.1</v>
+      </c>
+      <c r="H74">
+        <v>110903</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75">
+        <v>78290</v>
+      </c>
+      <c r="C75">
+        <v>78.40000000000001</v>
+      </c>
+      <c r="D75">
+        <v>359</v>
+      </c>
+      <c r="E75">
+        <v>0.4</v>
+      </c>
+      <c r="F75">
+        <v>21207</v>
+      </c>
+      <c r="G75">
+        <v>21.2</v>
+      </c>
+      <c r="H75">
+        <v>99856</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76">
+        <v>88866</v>
+      </c>
+      <c r="C76">
+        <v>78.7</v>
+      </c>
+      <c r="D76">
+        <v>360</v>
+      </c>
+      <c r="E76">
+        <v>0.3</v>
+      </c>
+      <c r="F76">
+        <v>23762</v>
+      </c>
+      <c r="G76">
+        <v>21</v>
+      </c>
+      <c r="H76">
+        <v>112988</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77">
+        <v>112712</v>
+      </c>
+      <c r="C77">
+        <v>80.5</v>
+      </c>
+      <c r="D77">
+        <v>377</v>
+      </c>
+      <c r="E77">
+        <v>0.3</v>
+      </c>
+      <c r="F77">
+        <v>26966</v>
+      </c>
+      <c r="G77">
+        <v>19.3</v>
+      </c>
+      <c r="H77">
+        <v>140055</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78">
+        <v>97979</v>
+      </c>
+      <c r="C78">
+        <v>81.09999999999999</v>
+      </c>
+      <c r="D78">
+        <v>372</v>
+      </c>
+      <c r="E78">
+        <v>0.3</v>
+      </c>
+      <c r="F78">
+        <v>22403</v>
+      </c>
+      <c r="G78">
+        <v>18.6</v>
+      </c>
+      <c r="H78">
+        <v>120754</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79">
+        <v>97126</v>
+      </c>
+      <c r="C79">
+        <v>82.7</v>
+      </c>
+      <c r="D79">
+        <v>182</v>
+      </c>
+      <c r="E79">
+        <v>0.2</v>
+      </c>
+      <c r="F79">
+        <v>20154</v>
+      </c>
+      <c r="G79">
+        <v>17.2</v>
+      </c>
+      <c r="H79">
+        <v>117462</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80">
+        <v>86112</v>
+      </c>
+      <c r="C80">
+        <v>82</v>
+      </c>
+      <c r="D80">
+        <v>198</v>
+      </c>
+      <c r="E80">
+        <v>0.2</v>
+      </c>
+      <c r="F80">
+        <v>18745</v>
+      </c>
+      <c r="G80">
+        <v>17.8</v>
+      </c>
+      <c r="H80">
+        <v>105055</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81">
+        <v>82763</v>
+      </c>
+      <c r="C81">
+        <v>83.8</v>
+      </c>
+      <c r="D81">
+        <v>258</v>
+      </c>
+      <c r="E81">
+        <v>0.3</v>
+      </c>
+      <c r="F81">
+        <v>15745</v>
+      </c>
+      <c r="G81">
+        <v>15.9</v>
+      </c>
+      <c r="H81">
+        <v>98766</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82">
+        <v>83657</v>
+      </c>
+      <c r="C82">
+        <v>79.2</v>
+      </c>
+      <c r="D82">
+        <v>357</v>
+      </c>
+      <c r="E82">
+        <v>0.3</v>
+      </c>
+      <c r="F82">
+        <v>21560</v>
+      </c>
+      <c r="G82">
+        <v>20.4</v>
+      </c>
+      <c r="H82">
+        <v>105574</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83">
+        <v>90392</v>
+      </c>
+      <c r="C83">
+        <v>79.59999999999999</v>
+      </c>
+      <c r="D83">
+        <v>357</v>
+      </c>
+      <c r="E83">
+        <v>0.3</v>
+      </c>
+      <c r="F83">
+        <v>22817</v>
+      </c>
+      <c r="G83">
+        <v>20.1</v>
+      </c>
+      <c r="H83">
+        <v>113566</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84">
+        <v>80869</v>
+      </c>
+      <c r="C84">
+        <v>81</v>
+      </c>
+      <c r="D84">
+        <v>343</v>
+      </c>
+      <c r="E84">
+        <v>0.3</v>
+      </c>
+      <c r="F84">
+        <v>18569</v>
+      </c>
+      <c r="G84">
+        <v>18.6</v>
+      </c>
+      <c r="H84">
+        <v>99781</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85">
+        <v>97849</v>
+      </c>
+      <c r="C85">
+        <v>82.7</v>
+      </c>
+      <c r="D85">
+        <v>250</v>
+      </c>
+      <c r="E85">
+        <v>0.2</v>
+      </c>
+      <c r="F85">
+        <v>20169</v>
+      </c>
+      <c r="G85">
+        <v>17.1</v>
+      </c>
+      <c r="H85">
+        <v>118268</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86">
+        <v>78627</v>
+      </c>
+      <c r="C86">
+        <v>76.40000000000001</v>
+      </c>
+      <c r="D86">
+        <v>256</v>
+      </c>
+      <c r="E86">
+        <v>0.2</v>
+      </c>
+      <c r="F86">
+        <v>23975</v>
+      </c>
+      <c r="G86">
+        <v>23.3</v>
+      </c>
+      <c r="H86">
+        <v>102858</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87">
+        <v>84030</v>
+      </c>
+      <c r="C87">
+        <v>82.2</v>
+      </c>
+      <c r="D87">
+        <v>209</v>
+      </c>
+      <c r="E87">
+        <v>0.2</v>
+      </c>
+      <c r="F87">
+        <v>17981</v>
+      </c>
+      <c r="G87">
+        <v>17.6</v>
+      </c>
+      <c r="H87">
+        <v>102220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88">
+        <v>86156</v>
+      </c>
+      <c r="C88">
+        <v>81.2</v>
+      </c>
+      <c r="D88">
+        <v>220</v>
+      </c>
+      <c r="E88">
+        <v>0.2</v>
+      </c>
+      <c r="F88">
+        <v>19691</v>
+      </c>
+      <c r="G88">
+        <v>18.6</v>
+      </c>
+      <c r="H88">
+        <v>106067</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89">
+        <v>91574</v>
+      </c>
+      <c r="C89">
+        <v>81.5</v>
+      </c>
+      <c r="D89">
+        <v>159</v>
+      </c>
+      <c r="E89">
+        <v>0.1</v>
+      </c>
+      <c r="F89">
+        <v>20656</v>
+      </c>
+      <c r="G89">
+        <v>18.4</v>
+      </c>
+      <c r="H89">
+        <v>112389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90">
+        <v>73834</v>
+      </c>
+      <c r="C90">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="D90">
+        <v>230</v>
+      </c>
+      <c r="E90">
+        <v>0.2</v>
+      </c>
+      <c r="F90">
+        <v>24896</v>
+      </c>
+      <c r="G90">
+        <v>25.2</v>
+      </c>
+      <c r="H90">
+        <v>98960</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>99</v>
+      </c>
+      <c r="B91">
+        <v>77138</v>
+      </c>
+      <c r="C91">
+        <v>74</v>
+      </c>
+      <c r="D91">
+        <v>205</v>
+      </c>
+      <c r="E91">
+        <v>0.2</v>
+      </c>
+      <c r="F91">
+        <v>26943</v>
+      </c>
+      <c r="G91">
+        <v>25.8</v>
+      </c>
+      <c r="H91">
+        <v>104286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92">
+        <v>83194</v>
+      </c>
+      <c r="C92">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="D92">
+        <v>190</v>
+      </c>
+      <c r="E92">
+        <v>0.2</v>
+      </c>
+      <c r="F92">
+        <v>18527</v>
+      </c>
+      <c r="G92">
+        <v>18.2</v>
+      </c>
+      <c r="H92">
+        <v>101911</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93">
+        <v>84372</v>
+      </c>
+      <c r="C93">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="D93">
+        <v>215</v>
+      </c>
+      <c r="E93">
+        <v>0.2</v>
+      </c>
+      <c r="F93">
+        <v>26234</v>
+      </c>
+      <c r="G93">
+        <v>23.7</v>
+      </c>
+      <c r="H93">
+        <v>110821</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94">
+        <v>90961</v>
+      </c>
+      <c r="C94">
+        <v>80.8</v>
+      </c>
+      <c r="D94">
+        <v>277</v>
+      </c>
+      <c r="E94">
+        <v>0.2</v>
+      </c>
+      <c r="F94">
+        <v>21335</v>
+      </c>
+      <c r="G94">
+        <v>19</v>
+      </c>
+      <c r="H94">
+        <v>112573</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>103</v>
+      </c>
+      <c r="B95">
+        <v>82806</v>
+      </c>
+      <c r="C95">
+        <v>80.59999999999999</v>
+      </c>
+      <c r="D95">
+        <v>258</v>
+      </c>
+      <c r="E95">
+        <v>0.3</v>
+      </c>
+      <c r="F95">
+        <v>19625</v>
+      </c>
+      <c r="G95">
+        <v>19.1</v>
+      </c>
+      <c r="H95">
+        <v>102689</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96">
+        <v>75803</v>
+      </c>
+      <c r="C96">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="D96">
+        <v>262</v>
+      </c>
+      <c r="E96">
+        <v>0.3</v>
+      </c>
+      <c r="F96">
+        <v>24529</v>
+      </c>
+      <c r="G96">
+        <v>24.4</v>
+      </c>
+      <c r="H96">
+        <v>100594</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97">
+        <v>77522</v>
+      </c>
+      <c r="C97">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="D97">
+        <v>231</v>
+      </c>
+      <c r="E97">
+        <v>0.2</v>
+      </c>
+      <c r="F97">
+        <v>24423</v>
+      </c>
+      <c r="G97">
+        <v>23.9</v>
+      </c>
+      <c r="H97">
+        <v>102176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98">
+        <v>90303</v>
+      </c>
+      <c r="C98">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="D98">
+        <v>184</v>
+      </c>
+      <c r="E98">
+        <v>0.2</v>
+      </c>
+      <c r="F98">
+        <v>20133</v>
+      </c>
+      <c r="G98">
+        <v>18.2</v>
+      </c>
+      <c r="H98">
+        <v>110620</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99">
+        <v>82451</v>
+      </c>
+      <c r="C99">
+        <v>79.7</v>
+      </c>
+      <c r="D99">
+        <v>262</v>
+      </c>
+      <c r="E99">
+        <v>0.3</v>
+      </c>
+      <c r="F99">
+        <v>20717</v>
+      </c>
+      <c r="G99">
+        <v>20</v>
+      </c>
+      <c r="H99">
+        <v>103430</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100">
+        <v>76551</v>
+      </c>
+      <c r="C100">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="D100">
+        <v>207</v>
+      </c>
+      <c r="E100">
+        <v>0.2</v>
+      </c>
+      <c r="F100">
+        <v>29665</v>
+      </c>
+      <c r="G100">
+        <v>27.9</v>
+      </c>
+      <c r="H100">
+        <v>106423</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101">
+        <v>80197</v>
+      </c>
+      <c r="C101">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="D101">
+        <v>308</v>
+      </c>
+      <c r="E101">
+        <v>0.3</v>
+      </c>
+      <c r="F101">
+        <v>22425</v>
+      </c>
+      <c r="G101">
+        <v>21.8</v>
+      </c>
+      <c r="H101">
+        <v>102930</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102">
+        <v>70944</v>
+      </c>
+      <c r="C102">
+        <v>70.2</v>
+      </c>
+      <c r="D102">
+        <v>263</v>
+      </c>
+      <c r="E102">
+        <v>0.3</v>
+      </c>
+      <c r="F102">
+        <v>29794</v>
+      </c>
+      <c r="G102">
+        <v>29.5</v>
+      </c>
+      <c r="H102">
+        <v>101001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103">
+        <v>75356</v>
+      </c>
+      <c r="C103">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="D103">
+        <v>239</v>
+      </c>
+      <c r="E103">
+        <v>0.2</v>
+      </c>
+      <c r="F103">
+        <v>35841</v>
+      </c>
+      <c r="G103">
+        <v>32.2</v>
+      </c>
+      <c r="H103">
+        <v>111436</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104">
+        <v>88662</v>
+      </c>
+      <c r="C104">
+        <v>81.2</v>
+      </c>
+      <c r="D104">
+        <v>218</v>
+      </c>
+      <c r="E104">
+        <v>0.2</v>
+      </c>
+      <c r="F104">
+        <v>20249</v>
+      </c>
+      <c r="G104">
+        <v>18.6</v>
+      </c>
+      <c r="H104">
+        <v>109129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105">
+        <v>84844</v>
+      </c>
+      <c r="C105">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="D105">
+        <v>258</v>
+      </c>
+      <c r="E105">
+        <v>0.2</v>
+      </c>
+      <c r="F105">
+        <v>24250</v>
+      </c>
+      <c r="G105">
+        <v>22.2</v>
+      </c>
+      <c r="H105">
+        <v>109352</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106">
+        <v>80783</v>
+      </c>
+      <c r="C106">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="D106">
+        <v>352</v>
+      </c>
+      <c r="E106">
+        <v>0.3</v>
+      </c>
+      <c r="F106">
+        <v>22553</v>
+      </c>
+      <c r="G106">
+        <v>21.8</v>
+      </c>
+      <c r="H106">
+        <v>103688</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107">
+        <v>82520</v>
+      </c>
+      <c r="C107">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="D107">
+        <v>229</v>
+      </c>
+      <c r="E107">
+        <v>0.2</v>
+      </c>
+      <c r="F107">
+        <v>23214</v>
+      </c>
+      <c r="G107">
+        <v>21.9</v>
+      </c>
+      <c r="H107">
+        <v>105963</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108">
+        <v>79283</v>
+      </c>
+      <c r="C108">
+        <v>75.7</v>
+      </c>
+      <c r="D108">
+        <v>214</v>
+      </c>
+      <c r="E108">
+        <v>0.2</v>
+      </c>
+      <c r="F108">
+        <v>25232</v>
+      </c>
+      <c r="G108">
+        <v>24.1</v>
+      </c>
+      <c r="H108">
+        <v>104729</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>117</v>
+      </c>
+      <c r="B109">
+        <v>77831</v>
+      </c>
+      <c r="C109">
+        <v>79.40000000000001</v>
+      </c>
+      <c r="D109">
+        <v>220</v>
+      </c>
+      <c r="E109">
+        <v>0.2</v>
+      </c>
+      <c r="F109">
+        <v>20020</v>
+      </c>
+      <c r="G109">
+        <v>20.4</v>
+      </c>
+      <c r="H109">
+        <v>98071</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110">
+        <v>74020</v>
+      </c>
+      <c r="C110">
+        <v>75.8</v>
+      </c>
+      <c r="D110">
+        <v>224</v>
+      </c>
+      <c r="E110">
+        <v>0.2</v>
+      </c>
+      <c r="F110">
+        <v>23348</v>
+      </c>
+      <c r="G110">
+        <v>23.9</v>
+      </c>
+      <c r="H110">
+        <v>97592</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111">
+        <v>86211</v>
+      </c>
+      <c r="C111">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="D111">
+        <v>200</v>
+      </c>
+      <c r="E111">
+        <v>0.2</v>
+      </c>
+      <c r="F111">
+        <v>23323</v>
+      </c>
+      <c r="G111">
+        <v>21.3</v>
+      </c>
+      <c r="H111">
+        <v>109734</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112">
+        <v>76191</v>
+      </c>
+      <c r="C112">
+        <v>74.3</v>
+      </c>
+      <c r="D112">
+        <v>237</v>
+      </c>
+      <c r="E112">
+        <v>0.2</v>
+      </c>
+      <c r="F112">
+        <v>26119</v>
+      </c>
+      <c r="G112">
+        <v>25.5</v>
+      </c>
+      <c r="H112">
+        <v>102547</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113">
+        <v>89418</v>
+      </c>
+      <c r="C113">
+        <v>84.5</v>
+      </c>
+      <c r="D113">
+        <v>162</v>
+      </c>
+      <c r="E113">
+        <v>0.2</v>
+      </c>
+      <c r="F113">
+        <v>16223</v>
+      </c>
+      <c r="G113">
+        <v>15.3</v>
+      </c>
+      <c r="H113">
+        <v>105803</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>122</v>
+      </c>
+      <c r="B114">
+        <v>83572</v>
+      </c>
+      <c r="C114">
+        <v>79.2</v>
+      </c>
+      <c r="D114">
+        <v>319</v>
+      </c>
+      <c r="E114">
+        <v>0.3</v>
+      </c>
+      <c r="F114">
+        <v>21645</v>
+      </c>
+      <c r="G114">
+        <v>20.5</v>
+      </c>
+      <c r="H114">
+        <v>105536</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>123</v>
+      </c>
+      <c r="B115">
+        <v>82921</v>
+      </c>
+      <c r="C115">
+        <v>78.7</v>
+      </c>
+      <c r="D115">
+        <v>280</v>
+      </c>
+      <c r="E115">
+        <v>0.3</v>
+      </c>
+      <c r="F115">
+        <v>22144</v>
+      </c>
+      <c r="G115">
+        <v>21</v>
+      </c>
+      <c r="H115">
+        <v>105345</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116">
+        <v>89540</v>
+      </c>
+      <c r="C116">
+        <v>81.2</v>
+      </c>
+      <c r="D116">
+        <v>217</v>
+      </c>
+      <c r="E116">
+        <v>0.2</v>
+      </c>
+      <c r="F116">
+        <v>20477</v>
+      </c>
+      <c r="G116">
+        <v>18.6</v>
+      </c>
+      <c r="H116">
+        <v>110234</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117">
+        <v>81325</v>
+      </c>
+      <c r="C117">
+        <v>76.8</v>
+      </c>
+      <c r="D117">
+        <v>243</v>
+      </c>
+      <c r="E117">
+        <v>0.2</v>
+      </c>
+      <c r="F117">
+        <v>24297</v>
+      </c>
+      <c r="G117">
+        <v>23</v>
+      </c>
+      <c r="H117">
+        <v>105865</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>126</v>
+      </c>
+      <c r="B118">
+        <v>90695</v>
+      </c>
+      <c r="C118">
+        <v>84.09999999999999</v>
+      </c>
+      <c r="D118">
+        <v>234</v>
+      </c>
+      <c r="E118">
+        <v>0.2</v>
+      </c>
+      <c r="F118">
+        <v>16919</v>
+      </c>
+      <c r="G118">
+        <v>15.7</v>
+      </c>
+      <c r="H118">
+        <v>107848</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>127</v>
+      </c>
+      <c r="B119">
+        <v>76561</v>
+      </c>
+      <c r="C119">
+        <v>75</v>
+      </c>
+      <c r="D119">
+        <v>260</v>
+      </c>
+      <c r="E119">
+        <v>0.3</v>
+      </c>
+      <c r="F119">
+        <v>25327</v>
+      </c>
+      <c r="G119">
+        <v>24.8</v>
+      </c>
+      <c r="H119">
+        <v>102148</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120">
+        <v>91560</v>
+      </c>
+      <c r="C120">
+        <v>81.5</v>
+      </c>
+      <c r="D120">
+        <v>273</v>
+      </c>
+      <c r="E120">
+        <v>0.2</v>
+      </c>
+      <c r="F120">
+        <v>20548</v>
+      </c>
+      <c r="G120">
+        <v>18.3</v>
+      </c>
+      <c r="H120">
+        <v>112381</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>129</v>
+      </c>
+      <c r="B121">
+        <v>86430</v>
+      </c>
+      <c r="C121">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="D121">
+        <v>252</v>
+      </c>
+      <c r="E121">
+        <v>0.2</v>
+      </c>
+      <c r="F121">
+        <v>20764</v>
+      </c>
+      <c r="G121">
+        <v>19.3</v>
+      </c>
+      <c r="H121">
+        <v>107446</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>130</v>
+      </c>
+      <c r="B122">
+        <v>85290</v>
+      </c>
+      <c r="C122">
+        <v>79.3</v>
+      </c>
+      <c r="D122">
+        <v>242</v>
+      </c>
+      <c r="E122">
+        <v>0.2</v>
+      </c>
+      <c r="F122">
+        <v>21991</v>
+      </c>
+      <c r="G122">
+        <v>20.5</v>
+      </c>
+      <c r="H122">
+        <v>107523</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123">
+        <v>88608</v>
+      </c>
+      <c r="C123">
+        <v>83.5</v>
+      </c>
+      <c r="D123">
+        <v>261</v>
+      </c>
+      <c r="E123">
+        <v>0.2</v>
+      </c>
+      <c r="F123">
+        <v>17239</v>
+      </c>
+      <c r="G123">
+        <v>16.2</v>
+      </c>
+      <c r="H123">
+        <v>106108</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124">
+        <v>87518</v>
+      </c>
+      <c r="C124">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="D124">
+        <v>276</v>
+      </c>
+      <c r="E124">
+        <v>0.2</v>
+      </c>
+      <c r="F124">
+        <v>27253</v>
+      </c>
+      <c r="G124">
+        <v>23.7</v>
+      </c>
+      <c r="H124">
+        <v>115047</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
+        <v>133</v>
+      </c>
+      <c r="B125">
+        <v>84963</v>
+      </c>
+      <c r="C125">
+        <v>81.2</v>
+      </c>
+      <c r="D125">
+        <v>252</v>
+      </c>
+      <c r="E125">
+        <v>0.2</v>
+      </c>
+      <c r="F125">
+        <v>19410</v>
+      </c>
+      <c r="G125">
+        <v>18.6</v>
+      </c>
+      <c r="H125">
+        <v>104625</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
+        <v>134</v>
+      </c>
+      <c r="B126">
+        <v>86285</v>
+      </c>
+      <c r="C126">
+        <v>75.5</v>
+      </c>
+      <c r="D126">
+        <v>268</v>
+      </c>
+      <c r="E126">
+        <v>0.2</v>
+      </c>
+      <c r="F126">
+        <v>27802</v>
+      </c>
+      <c r="G126">
+        <v>24.3</v>
+      </c>
+      <c r="H126">
+        <v>114355</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>135</v>
+      </c>
+      <c r="B127">
+        <v>77434</v>
+      </c>
+      <c r="C127">
+        <v>75.8</v>
+      </c>
+      <c r="D127">
+        <v>194</v>
+      </c>
+      <c r="E127">
+        <v>0.2</v>
+      </c>
+      <c r="F127">
+        <v>24466</v>
+      </c>
+      <c r="G127">
+        <v>24</v>
+      </c>
+      <c r="H127">
+        <v>102094</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>136</v>
+      </c>
+      <c r="B128">
+        <v>77333</v>
+      </c>
+      <c r="C128">
+        <v>76</v>
+      </c>
+      <c r="D128">
+        <v>169</v>
+      </c>
+      <c r="E128">
+        <v>0.2</v>
+      </c>
+      <c r="F128">
+        <v>24197</v>
+      </c>
+      <c r="G128">
+        <v>23.8</v>
+      </c>
+      <c r="H128">
+        <v>101699</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>137</v>
+      </c>
+      <c r="B129">
+        <v>80505</v>
+      </c>
+      <c r="C129">
+        <v>78.3</v>
+      </c>
+      <c r="D129">
+        <v>214</v>
+      </c>
+      <c r="E129">
+        <v>0.2</v>
+      </c>
+      <c r="F129">
+        <v>22157</v>
+      </c>
+      <c r="G129">
+        <v>21.5</v>
+      </c>
+      <c r="H129">
+        <v>102876</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130">
+        <v>75463</v>
+      </c>
+      <c r="C130">
+        <v>77.8</v>
+      </c>
+      <c r="D130">
+        <v>184</v>
+      </c>
+      <c r="E130">
+        <v>0.2</v>
+      </c>
+      <c r="F130">
+        <v>21330</v>
+      </c>
+      <c r="G130">
+        <v>22</v>
+      </c>
+      <c r="H130">
+        <v>96977</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>139</v>
+      </c>
+      <c r="B131">
+        <v>82581</v>
+      </c>
+      <c r="C131">
+        <v>83.90000000000001</v>
+      </c>
+      <c r="D131">
+        <v>178</v>
+      </c>
+      <c r="E131">
+        <v>0.2</v>
+      </c>
+      <c r="F131">
+        <v>15706</v>
+      </c>
+      <c r="G131">
+        <v>16</v>
+      </c>
+      <c r="H131">
+        <v>98465</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>140</v>
+      </c>
+      <c r="B132">
+        <v>66432</v>
+      </c>
+      <c r="C132">
+        <v>67.8</v>
+      </c>
+      <c r="D132">
+        <v>194</v>
+      </c>
+      <c r="E132">
+        <v>0.2</v>
+      </c>
+      <c r="F132">
+        <v>31428</v>
+      </c>
+      <c r="G132">
+        <v>32.1</v>
+      </c>
+      <c r="H132">
+        <v>98054</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>141</v>
+      </c>
+      <c r="B133">
+        <v>80897</v>
+      </c>
+      <c r="C133">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="D133">
+        <v>225</v>
+      </c>
+      <c r="E133">
+        <v>0.2</v>
+      </c>
+      <c r="F133">
+        <v>21752</v>
+      </c>
+      <c r="G133">
+        <v>21.1</v>
+      </c>
+      <c r="H133">
+        <v>102874</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>142</v>
+      </c>
+      <c r="B134">
+        <v>82100</v>
+      </c>
+      <c r="C134">
+        <v>80.3</v>
+      </c>
+      <c r="D134">
+        <v>236</v>
+      </c>
+      <c r="E134">
+        <v>0.2</v>
+      </c>
+      <c r="F134">
+        <v>19878</v>
+      </c>
+      <c r="G134">
+        <v>19.4</v>
+      </c>
+      <c r="H134">
+        <v>102214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>143</v>
+      </c>
+      <c r="B135">
+        <v>76716</v>
+      </c>
+      <c r="C135">
+        <v>79.5</v>
+      </c>
+      <c r="D135">
+        <v>230</v>
+      </c>
+      <c r="E135">
+        <v>0.2</v>
+      </c>
+      <c r="F135">
+        <v>19570</v>
+      </c>
+      <c r="G135">
+        <v>20.3</v>
+      </c>
+      <c r="H135">
+        <v>96516</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+      <c r="B136">
+        <v>83380</v>
+      </c>
+      <c r="C136">
+        <v>83</v>
+      </c>
+      <c r="D136">
+        <v>195</v>
+      </c>
+      <c r="E136">
+        <v>0.2</v>
+      </c>
+      <c r="F136">
+        <v>16916</v>
+      </c>
+      <c r="G136">
+        <v>16.8</v>
+      </c>
+      <c r="H136">
+        <v>100491</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>145</v>
+      </c>
+      <c r="B137">
+        <v>77541</v>
+      </c>
+      <c r="C137">
+        <v>75.5</v>
+      </c>
+      <c r="D137">
+        <v>234</v>
+      </c>
+      <c r="E137">
+        <v>0.2</v>
+      </c>
+      <c r="F137">
+        <v>24925</v>
+      </c>
+      <c r="G137">
+        <v>24.3</v>
+      </c>
+      <c r="H137">
+        <v>102700</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>146</v>
+      </c>
+      <c r="B138">
+        <v>85004</v>
+      </c>
+      <c r="C138">
+        <v>76.2</v>
+      </c>
+      <c r="D138">
+        <v>209</v>
+      </c>
+      <c r="E138">
+        <v>0.2</v>
+      </c>
+      <c r="F138">
+        <v>26401</v>
+      </c>
+      <c r="G138">
+        <v>23.7</v>
+      </c>
+      <c r="H138">
+        <v>111614</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>147</v>
+      </c>
+      <c r="B139">
+        <v>80477</v>
+      </c>
+      <c r="C139">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="D139">
+        <v>177</v>
+      </c>
+      <c r="E139">
+        <v>0.2</v>
+      </c>
+      <c r="F139">
+        <v>19479</v>
+      </c>
+      <c r="G139">
+        <v>19.5</v>
+      </c>
+      <c r="H139">
+        <v>100133</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>148</v>
+      </c>
+      <c r="B140">
+        <v>77285</v>
+      </c>
+      <c r="C140">
+        <v>78.2</v>
+      </c>
+      <c r="D140">
+        <v>190</v>
+      </c>
+      <c r="E140">
+        <v>0.2</v>
+      </c>
+      <c r="F140">
+        <v>21345</v>
+      </c>
+      <c r="G140">
+        <v>21.6</v>
+      </c>
+      <c r="H140">
+        <v>98820</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>149</v>
+      </c>
+      <c r="B141">
+        <v>75923</v>
+      </c>
+      <c r="C141">
+        <v>77.5</v>
+      </c>
+      <c r="D141">
+        <v>185</v>
+      </c>
+      <c r="E141">
+        <v>0.2</v>
+      </c>
+      <c r="F141">
+        <v>21857</v>
+      </c>
+      <c r="G141">
+        <v>22.3</v>
+      </c>
+      <c r="H141">
+        <v>97965</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>150</v>
+      </c>
+      <c r="B142">
+        <v>78428</v>
+      </c>
+      <c r="C142">
+        <v>83.90000000000001</v>
+      </c>
+      <c r="D142">
+        <v>174</v>
+      </c>
+      <c r="E142">
+        <v>0.2</v>
+      </c>
+      <c r="F142">
+        <v>14926</v>
+      </c>
+      <c r="G142">
+        <v>16</v>
+      </c>
+      <c r="H142">
+        <v>93528</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>151</v>
+      </c>
+      <c r="B143">
+        <v>58759</v>
+      </c>
+      <c r="C143">
+        <v>79</v>
+      </c>
+      <c r="D143">
+        <v>145</v>
+      </c>
+      <c r="E143">
+        <v>0.2</v>
+      </c>
+      <c r="F143">
+        <v>15487</v>
+      </c>
+      <c r="G143">
+        <v>20.8</v>
+      </c>
+      <c r="H143">
+        <v>74391</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>152</v>
+      </c>
+      <c r="B144">
+        <v>55627</v>
+      </c>
+      <c r="C144">
+        <v>75.8</v>
+      </c>
+      <c r="D144">
+        <v>154</v>
+      </c>
+      <c r="E144">
+        <v>0.2</v>
+      </c>
+      <c r="F144">
+        <v>17632</v>
+      </c>
+      <c r="G144">
+        <v>24</v>
+      </c>
+      <c r="H144">
+        <v>73413</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>153</v>
+      </c>
+      <c r="B145">
+        <v>60997</v>
+      </c>
+      <c r="C145">
+        <v>82.09999999999999</v>
+      </c>
+      <c r="D145">
+        <v>167</v>
+      </c>
+      <c r="E145">
+        <v>0.2</v>
+      </c>
+      <c r="F145">
+        <v>13092</v>
+      </c>
+      <c r="G145">
+        <v>17.6</v>
+      </c>
+      <c r="H145">
+        <v>74256</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>154</v>
+      </c>
+      <c r="B146">
+        <v>65068</v>
+      </c>
+      <c r="C146">
+        <v>82.5</v>
+      </c>
+      <c r="D146">
+        <v>163</v>
+      </c>
+      <c r="E146">
+        <v>0.2</v>
+      </c>
+      <c r="F146">
+        <v>13605</v>
+      </c>
+      <c r="G146">
+        <v>17.3</v>
+      </c>
+      <c r="H146">
+        <v>78836</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>155</v>
+      </c>
+      <c r="B147">
+        <v>61152</v>
+      </c>
+      <c r="C147">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="D147">
+        <v>176</v>
+      </c>
+      <c r="E147">
+        <v>0.2</v>
+      </c>
+      <c r="F147">
+        <v>17204</v>
+      </c>
+      <c r="G147">
+        <v>21.9</v>
+      </c>
+      <c r="H147">
+        <v>78532</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>156</v>
+      </c>
+      <c r="B148">
+        <v>34924</v>
+      </c>
+      <c r="C148">
+        <v>50</v>
+      </c>
+      <c r="D148">
+        <v>106</v>
+      </c>
+      <c r="E148">
+        <v>0.2</v>
+      </c>
+      <c r="F148">
+        <v>34854</v>
+      </c>
+      <c r="G148">
+        <v>49.9</v>
+      </c>
+      <c r="H148">
+        <v>69884</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>157</v>
+      </c>
+      <c r="B149">
+        <v>45452</v>
+      </c>
+      <c r="C149">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="D149">
+        <v>123</v>
+      </c>
+      <c r="E149">
+        <v>0.2</v>
+      </c>
+      <c r="F149">
+        <v>22642</v>
+      </c>
+      <c r="G149">
+        <v>33.2</v>
+      </c>
+      <c r="H149">
+        <v>68217</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150">
+        <v>120951</v>
+      </c>
+      <c r="C150">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="D150">
+        <v>281</v>
+      </c>
+      <c r="E150">
+        <v>0.2</v>
+      </c>
+      <c r="F150">
+        <v>24399</v>
+      </c>
+      <c r="G150">
+        <v>16.8</v>
+      </c>
+      <c r="H150">
+        <v>145631</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>159</v>
+      </c>
+      <c r="B151">
+        <v>116028</v>
+      </c>
+      <c r="C151">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="D151">
+        <v>253</v>
+      </c>
+      <c r="E151">
+        <v>0.2</v>
+      </c>
+      <c r="F151">
+        <v>26196</v>
+      </c>
+      <c r="G151">
+        <v>18.4</v>
+      </c>
+      <c r="H151">
+        <v>142477</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>